<commit_message>
OC Cascade Delete Test Automation
</commit_message>
<xml_diff>
--- a/automation/RobotFrameworkAutomation/Regression/TestData/OC/OC_Data.xlsx
+++ b/automation/RobotFrameworkAutomation/Regression/TestData/OC/OC_Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,26 @@
           <t>TC10</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>TC11</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>TC12</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>TC13</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>TC14</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -556,6 +576,26 @@
           <t>Service Order for Operator Connect</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Service Order for Operator Connect</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Service Order for Operator Connect</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Service Order for Operator Connect</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Service Order for Operator Connect</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -618,6 +658,26 @@
           <t>OC Regression</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>OC Regression</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>OC Regression</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>OC Regression</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>OC Regression</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -680,6 +740,26 @@
           <t>BSS-Simulator</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>BSS-Simulator</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>BSS-Simulator</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>BSS-Simulator</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>BSS-Simulator</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -739,7 +819,27 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>TC09</t>
+          <t>TC10</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>TC11</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>TC12</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>TC13</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>TC14</t>
         </is>
       </c>
     </row>
@@ -800,6 +900,26 @@
         </is>
       </c>
       <c r="L6" t="inlineStr">
+        <is>
+          <t>55aa1f7f-2c04-4e16-8298-f2ea7f8aab99</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>55aa1f7f-2c04-4e16-8298-f2ea7f8aab99</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>55aa1f7f-2c04-4e16-8298-f2ea7f8aab99</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>55aa1f7f-2c04-4e16-8298-f2ea7f8aab99</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
         <is>
           <t>55aa1f7f-2c04-4e16-8298-f2ea7f8aab99</t>
         </is>
@@ -854,6 +974,10 @@
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -914,6 +1038,26 @@
       <c r="L8" t="inlineStr">
         <is>
           <t>OCTestMobileNumber</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>OCTestNumber</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>OCTestNumber</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>OCTestNumber</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>OCTestNumber</t>
         </is>
       </c>
     </row>
@@ -958,6 +1102,26 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -996,6 +1160,10 @@
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1018,6 +1186,10 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1040,6 +1212,10 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1054,22 +1230,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>RL10028701</t>
+          <t>RL10028799</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>RL10028702</t>
+          <t>RL10028800</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RL0009074</t>
+          <t>RL10028801</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>RL10028704</t>
+          <t>RL10028802</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1094,12 +1270,32 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>RL10028704</t>
+          <t>RL10028802</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>RL10028704</t>
+          <t>RL10028802</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>RL10028712</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>RL10028712</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>RL10028712</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>RL10028712</t>
         </is>
       </c>
     </row>
@@ -1116,22 +1312,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>31202007906</t>
+          <t>31208523339</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>31202007907</t>
+          <t>31208523340</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>31208000101</t>
+          <t>31208523341</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>31109051122</t>
+          <t>31109051126</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1143,10 +1339,30 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>31109051122</v>
+        <v>31109051126</v>
       </c>
       <c r="L14" t="n">
-        <v>31109051122</v>
+        <v>31109051126</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>31202007617</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>31202007617</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>31202007617</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>31202007617</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1206,6 +1422,26 @@
         </is>
       </c>
       <c r="L15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1236,6 +1472,10 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1250,22 +1490,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4262765442</t>
+          <t>4294144637</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4262762640</t>
+          <t>4294149965</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4228288896</t>
+          <t>4294154255</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4228288896</t>
+          <t>4294154255</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1274,6 +1514,26 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>4269197485</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>4269197485</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>4269197485</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>4269197485</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1288,38 +1548,38 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4262765445</t>
+          <t>4294144640</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4262762643</t>
+          <t>4294149968</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4228288899</t>
+          <t>4294154258</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>4228288899</t>
+          <t>4294154258</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>4228288899</t>
+          <t>4294154258</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>4228288899</t>
+          <t>4294154258</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>4228288899</t>
+          <t>4294154258</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1328,6 +1588,26 @@
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>4269197488</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>4269197488</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>4269197488</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>4269197488</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1342,22 +1622,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4262765449</t>
+          <t>4294144644</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4262762647</t>
+          <t>4294149972</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4228288903</t>
+          <t>4294154262</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4263541518</t>
+          <t>4294151459</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1366,12 +1646,32 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>4263541518</t>
+          <t>4294151459</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>4263541518</t>
+          <t>4294151459</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>4269197492</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>4269197492</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>4269197492</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>4269197492</t>
         </is>
       </c>
     </row>
@@ -1390,7 +1690,7 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>31109051122</v>
+        <v>31109051126</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -1398,8 +1698,12 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="n">
-        <v>31109051122</v>
-      </c>
+        <v>31109051126</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1438,6 +1742,26 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>01414155</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>01414155</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>01414155</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>01414155</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1462,6 +1786,10 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1479,7 +1807,7 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>4263541515</t>
+          <t>4294151456</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1488,6 +1816,10 @@
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1509,9 +1841,13 @@
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
-        <v>31109051122</v>
+        <v>31109051126</v>
       </c>
       <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1536,6 +1872,10 @@
         <v>1</v>
       </c>
       <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>